<commit_message>
Correction of each graph, colours and complete tibbles
</commit_message>
<xml_diff>
--- a/Parameters_DNAs.xlsx
+++ b/Parameters_DNAs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bringaf/Documents/Postdoc/Diffley/bioinformatics_programming/Github/NSONAR/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bringaf/Documents/Postdoc/Diffley/bioinformatics_programming/Github/Analysis_NS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6693F0BB-56A4-D642-8B73-507C76BFB08F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A892F2-2786-4944-8DBA-ADDF6631371A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="1760" windowWidth="27040" windowHeight="16860" xr2:uid="{AF07CA71-8B9C-D644-8284-8704F4EAC862}"/>
+    <workbookView xWindow="3200" yWindow="2780" windowWidth="27040" windowHeight="16860" xr2:uid="{AF07CA71-8B9C-D644-8284-8704F4EAC862}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
   <si>
     <t>Data: 50fmol ~3M reads</t>
   </si>
@@ -150,18 +150,12 @@
     <t>DNAscent_T5</t>
   </si>
   <si>
-    <t>no specified</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
     <t>37 H</t>
   </si>
   <si>
-    <t>11H</t>
-  </si>
-  <si>
     <t>DNAscent_T6</t>
   </si>
   <si>
@@ -171,70 +165,43 @@
     <t>Time stimated to finish (after 30 min started)</t>
   </si>
   <si>
-    <t>10H</t>
-  </si>
-  <si>
-    <t>20 H</t>
-  </si>
-  <si>
-    <t>#! /usr/bin/bash
-#SBATCH --job-name=T6
-#SBATCH --ntasks=1
-#SBATCH --cpus-per-task=32
-#SBATCH --mem=256G
-#SBATCH --gres=gpu:1
-#SBATCH --time=72:00:0
-#SBATCH --partition=gpu
-#SBATCH --output=std/dnascent_T6.o
-#SBATCH --error=std/dnascent_T6.e</t>
-  </si>
-  <si>
     <t>DNAscent_T7</t>
   </si>
   <si>
-    <t>#! /usr/bin/bash
-#SBATCH --job-name=T7
-#SBATCH --ntasks=1
-#SBATCH --cpus-per-task=32
-#SBATCH --gres=gpu:1
-#SBATCH --time=72:00:0
-#SBATCH --partition=gpu
-#SBATCH --output=std/dnascent_T7.o
-#SBATCH --error=std/dnascent_T7.e</t>
-  </si>
-  <si>
-    <t>DNAscent_T8</t>
-  </si>
-  <si>
-    <t>#! /usr/bin/bash
-#SBATCH --job-name=T8
-#SBATCH --ntasks=1
-#SBATCH --cpus-per-task=20
-#SBATCH --gres=gpu:1
-#SBATCH --time=72:00:0
-#SBATCH --partition=gpu
-#SBATCH --output=std/dnascent_T8.o
-#SBATCH --error=std/dnascent_T8.e</t>
+    <t>5H</t>
   </si>
   <si>
     <t>#! /usr/bin/bash
 #SBATCH --job-name=T5
 #SBATCH --ntasks=1
 #SBATCH --cpus-per-task=32
+#SBATCH --time=72:00:0
+#SBATCH --partition=ncpu
+#SBATCH --output=std/dnascent_T1.o
+#SBATCH --error=std/dnascent_T1.e</t>
+  </si>
+  <si>
+    <t>#! /usr/bin/bash
+#SBATCH --job-name=T6
+#SBATCH --ntasks=1
+#SBATCH --cpus-per-task=12
 #SBATCH --gres=gpu:1
-#SBATCH --time=10:00:0
+#SBATCH --time=16:00:0
 #SBATCH --partition=gpu
-#SBATCH --output=std/dnascent_T5.o
-#SBATCH --error=std/dnascent_T5.e</t>
-  </si>
-  <si>
-    <t>DNAscent_T9</t>
-  </si>
-  <si>
-    <t>5H</t>
-  </si>
-  <si>
-    <t>It’s the fastest so far</t>
+#SBATCH --output=std/dnascent_T6.o
+#SBATCH --error=std/dnascent_T6.e</t>
+  </si>
+  <si>
+    <t>128G</t>
+  </si>
+  <si>
+    <t>2 H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2H </t>
+  </si>
+  <si>
+    <t>Fastest</t>
   </si>
 </sst>
 </file>
@@ -625,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3423A777-E243-D34A-97B2-60063AE06565}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -667,10 +634,10 @@
         <v>15</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>6</v>
@@ -782,137 +749,87 @@
         <v>23</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" ht="153" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="136" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C8" s="1">
         <v>32</v>
       </c>
       <c r="D8" s="1">
-        <v>64</v>
+        <v>10</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" ht="170" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="153" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="1">
+        <v>10</v>
+      </c>
+      <c r="D9" s="1">
+        <v>10</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="1">
-        <v>32</v>
-      </c>
-      <c r="D9" s="1">
-        <v>64</v>
-      </c>
-      <c r="E9" s="1">
-        <v>256</v>
-      </c>
       <c r="F9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" ht="153" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C10" s="1">
         <v>32</v>
       </c>
       <c r="D10" s="1">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" ht="153" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="1">
-        <v>20</v>
-      </c>
-      <c r="D11" s="1">
-        <v>32</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" ht="136" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="1">
-        <v>32</v>
-      </c>
-      <c r="D12" s="1">
-        <v>10</v>
-      </c>
-      <c r="E12" s="1">
-        <v>256</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>